<commit_message>
stores wins and losses as observations and outputs totals
</commit_message>
<xml_diff>
--- a/OverwatchRankStats.xlsx
+++ b/OverwatchRankStats.xlsx
@@ -14,12 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
-    <t>totalLost</t>
+    <t>Win/Loss/Draw</t>
   </si>
   <si>
-    <t>totalWon</t>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>win</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>nan</t>
   </si>
 </sst>
 </file>
@@ -377,18 +386,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:C1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tank specific wins/losses
</commit_message>
<xml_diff>
--- a/OverwatchRankStats.xlsx
+++ b/OverwatchRankStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Win/Loss/Draw</t>
   </si>
@@ -22,13 +22,19 @@
     <t>Role</t>
   </si>
   <si>
+    <t>loss</t>
+  </si>
+  <si>
     <t>win</t>
   </si>
   <si>
-    <t>loss</t>
-  </si>
-  <si>
-    <t>nan</t>
+    <t>tank</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>support</t>
   </si>
 </sst>
 </file>
@@ -386,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -407,13 +413,19 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -421,7 +433,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -431,6 +446,9 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
@@ -441,6 +459,22 @@
       </c>
       <c r="C6" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted some unnecessary comments
</commit_message>
<xml_diff>
--- a/OverwatchRankStats.xlsx
+++ b/OverwatchRankStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Win/Loss/Draw</t>
   </si>
@@ -22,19 +22,10 @@
     <t>Role</t>
   </si>
   <si>
-    <t>loss</t>
-  </si>
-  <si>
     <t>win</t>
   </si>
   <si>
-    <t>tank</t>
-  </si>
-  <si>
     <t>damage</t>
-  </si>
-  <si>
-    <t>support</t>
   </si>
 </sst>
 </file>
@@ -392,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,67 +405,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
idk what this is
</commit_message>
<xml_diff>
--- a/OverwatchRankStats.xlsx
+++ b/OverwatchRankStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Win/Loss/Draw</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>win</t>
+  </si>
+  <si>
+    <t>nan</t>
   </si>
   <si>
     <t>damage</t>
@@ -383,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,7 +408,18 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exit button, see stats button, and started working on add game button
</commit_message>
<xml_diff>
--- a/OverwatchRankStats.xlsx
+++ b/OverwatchRankStats.xlsx
@@ -1,41 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jrous\GitHub\Overwatch-Rank-Tracker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95F8CB3-4D36-4461-B168-483E56181E0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1200" yWindow="0" windowWidth="21600" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
-  <si>
-    <t>Win/Loss/Draw</t>
-  </si>
-  <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>win</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>damage</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +88,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -144,7 +142,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,9 +174,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -210,6 +226,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -385,42 +419,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added some more roles
</commit_message>
<xml_diff>
--- a/OverwatchRankStats.xlsx
+++ b/OverwatchRankStats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Win/Loss/Draw</t>
   </si>
@@ -22,13 +22,19 @@
     <t>Role</t>
   </si>
   <si>
+    <t>loss</t>
+  </si>
+  <si>
     <t>win</t>
   </si>
   <si>
-    <t>loss</t>
-  </si>
-  <si>
-    <t>nan</t>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>DPS</t>
+  </si>
+  <si>
+    <t>Tank</t>
   </si>
 </sst>
 </file>
@@ -386,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -404,8 +410,8 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -413,10 +419,26 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>